<commit_message>
Updating visualizations, adding menu
</commit_message>
<xml_diff>
--- a/CourseSchema-ferran.xlsx
+++ b/CourseSchema-ferran.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="CourseCatalog" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="190">
   <si>
     <t xml:space="preserve">CourseCatalogID</t>
   </si>
@@ -346,6 +346,9 @@
     <t xml:space="preserve">TopicsID</t>
   </si>
   <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parent</t>
   </si>
   <si>
@@ -355,6 +358,12 @@
     <t xml:space="preserve">ShortName</t>
   </si>
   <si>
+    <t xml:space="preserve">Temple CIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS Core</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROOT</t>
   </si>
   <si>
@@ -376,6 +385,9 @@
     <t xml:space="preserve">Derivatives</t>
   </si>
   <si>
+    <t xml:space="preserve">CS Electives</t>
+  </si>
+  <si>
     <t xml:space="preserve">Partial Derivative</t>
   </si>
   <si>
@@ -391,6 +403,12 @@
     <t xml:space="preserve">Spanning Tree</t>
   </si>
   <si>
+    <t xml:space="preserve">KA Core</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logistics Regression</t>
+  </si>
+  <si>
     <t xml:space="preserve">CourseID</t>
   </si>
   <si>
@@ -427,9 +445,6 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
@@ -566,6 +581,24 @@
   </si>
   <si>
     <t xml:space="preserve">parent_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select one of the following:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select at most three Big Data courses from the following: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select a total of 15 credits, taking into account the following restrictions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select at most three Data Analysis courses from the following: </t>
   </si>
 </sst>
 </file>
@@ -641,7 +674,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -656,6 +689,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -677,11 +714,11 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O74" activeCellId="0" sqref="O74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.7"/>
@@ -2987,16 +3024,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="61.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3004,29 +3042,41 @@
         <v>14</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>183</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1001</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1002</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1003</v>
       </c>
@@ -3036,8 +3086,14 @@
       <c r="C4" s="0" t="n">
         <v>1005</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1004</v>
       </c>
@@ -3047,8 +3103,14 @@
       <c r="C5" s="0" t="n">
         <v>1005</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1005</v>
       </c>
@@ -3075,10 +3137,10 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.42"/>
@@ -3232,7 +3294,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3255,7 +3317,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.42"/>
@@ -3340,21 +3402,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>104</v>
       </c>
@@ -3362,15 +3427,21 @@
         <v>105</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3379,13 +3450,22 @@
         <v>1001</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>109</v>
+      <c r="F2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1052</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,13 +3473,22 @@
         <v>1002</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>110</v>
+      <c r="F3" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1053</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3407,13 +3496,22 @@
         <v>1003</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>111</v>
+      <c r="F4" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1054</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,13 +3519,22 @@
         <v>1004</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="D5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>112</v>
+      <c r="F5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1055</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,13 +3542,22 @@
         <v>1005</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2000</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>113</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1056</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,13 +3565,22 @@
         <v>1006</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>114</v>
+      <c r="F7" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1057</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,13 +3588,22 @@
         <v>1007</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>115</v>
+      <c r="F8" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1058</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3477,13 +3611,22 @@
         <v>1008</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>116</v>
+      <c r="F9" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1059</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,13 +3634,22 @@
         <v>1009</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>117</v>
+      <c r="F10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1060</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,13 +3657,22 @@
         <v>1010</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>118</v>
+      <c r="F11" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1061</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,13 +3680,42 @@
         <v>1011</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>119</v>
+      <c r="F12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1012</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3547,10 +3737,10 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
@@ -3559,27 +3749,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>104</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -3588,12 +3778,12 @@
         <v>2.6</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -3602,47 +3792,47 @@
         <v>9.1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3663,68 +3853,69 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.36328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="44.3359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="44.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="44.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="25.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="15.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="44.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="15.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="22.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="3" width="44.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="10" style="3" width="44.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>104</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1001</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>1001</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,16 +3923,16 @@
         <v>1002</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>1001</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3749,16 +3940,16 @@
         <v>1003</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>1001</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3766,16 +3957,16 @@
         <v>1004</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>1001</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3783,153 +3974,153 @@
         <v>1005</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>1006</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>1007</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>1004</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>1008</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>1004</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>1009</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>1008</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
         <v>1010</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>1008</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>1011</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <v>1012</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3954,7 +4145,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.3"/>
@@ -3971,28 +4162,28 @@
         <v>4</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,14 +4191,14 @@
         <v>1001</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4015,50 +4206,50 @@
         <v>1002</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4083,23 +4274,23 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4107,13 +4298,13 @@
         <v>1001</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4121,13 +4312,13 @@
         <v>1002</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>